<commit_message>
modify Best_result.xlsx column name
</commit_message>
<xml_diff>
--- a/examples/result/Best_result.xlsx
+++ b/examples/result/Best_result.xlsx
@@ -55,10 +55,10 @@
     <t>Best Test Result Metric 2</t>
   </si>
   <si>
-    <t>Difference 1</t>
-  </si>
-  <si>
-    <t>Difference 2</t>
+    <t>Full sample - FewShot(val)</t>
+  </si>
+  <si>
+    <t>Full sample - FewShot(test)</t>
   </si>
   <si>
     <t>[kaggle]Analytics Vidhya Loan Prediction</t>

</xml_diff>